<commit_message>
More and more and more
</commit_message>
<xml_diff>
--- a/critical-from-2019-2.xlsx
+++ b/critical-from-2019-2.xlsx
@@ -1,37 +1,111 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>промежуток</t>
+  </si>
+  <si>
+    <t>критическая_дата</t>
+  </si>
+  <si>
+    <t>0-100м</t>
+  </si>
+  <si>
+    <t>100-200м</t>
+  </si>
+  <si>
+    <t>200-300м</t>
+  </si>
+  <si>
+    <t>300-400м</t>
+  </si>
+  <si>
+    <t>400-500м</t>
+  </si>
+  <si>
+    <t>500-600м</t>
+  </si>
+  <si>
+    <t>600-700м</t>
+  </si>
+  <si>
+    <t>700-800м</t>
+  </si>
+  <si>
+    <t>800-900м</t>
+  </si>
+  <si>
+    <t>900-1000м</t>
+  </si>
+  <si>
+    <t>8-2024</t>
+  </si>
+  <si>
+    <t>6-2029</t>
+  </si>
+  <si>
+    <t>6-2022</t>
+  </si>
+  <si>
+    <t>6-2026</t>
+  </si>
+  <si>
+    <t>8-2023</t>
+  </si>
+  <si>
+    <t>5-2023</t>
+  </si>
+  <si>
+    <t>2-2021</t>
+  </si>
+  <si>
+    <t>5-2020</t>
+  </si>
+  <si>
+    <t>7-2020</t>
+  </si>
+  <si>
+    <t>3-2039</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,26 +120,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -353,167 +436,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>промежуток</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>критическая_дата</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0-100м</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>11-1920</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>100-200м</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>13-2019</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>200-300м</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>12-2016</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>300-400м</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>7-2019</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>400-500м</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>13-2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>500-600м</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>10-1920</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>600-700м</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>13-2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>700-800м</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>12-2034</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>800-900м</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>5-2019</t>
-        </is>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>